<commit_message>
Atualização dos dados e criação do excel total.
</commit_message>
<xml_diff>
--- a/oeb_taxa_de_cambio.xlsx
+++ b/oeb_taxa_de_cambio.xlsx
@@ -408,10 +408,10 @@
         <v>44743</v>
       </c>
       <c r="B2" t="n">
-        <v>5.3136</v>
+        <v>5.3084</v>
       </c>
       <c r="C2" t="n">
-        <v>0.0525</v>
+        <v>0.0515</v>
       </c>
     </row>
     <row r="3">
@@ -2094,10 +2094,10 @@
         <v>44743</v>
       </c>
       <c r="B2" t="n">
-        <v>5.5304</v>
+        <v>5.5295</v>
       </c>
       <c r="C2" t="n">
-        <v>0.0371</v>
+        <v>0.0369</v>
       </c>
     </row>
     <row r="3">

</xml_diff>